<commit_message>
save info in xl
</commit_message>
<xml_diff>
--- a/blog_automatic_posting.xlsx
+++ b/blog_automatic_posting.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,27 +437,104 @@
           <t>best_review</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>온방바닥에 실밥 천지고 실밥정리가 전혀안되있어요 털어봐도 어디서나오는지 계속나와요 ㅠ
-허리띠는 짧아서 쓸수도 없어요
-ㅠ</t>
+          <t>https://link.coupang.com/a/cmgjus</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>http://thumbnail7.coupangcdn.com/thumbnails/remote/292x292ex/image/vendor_inventory/065f/32cfe83ec2d5f60dd258b5d5e109abc004e5ebaafe3e72064ff23e7ab855.jpg</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>빠른 배송 감사합니다
+인터넷 쇼핑으로 의류를 구매하고 실망한 경험이 있었는데 만족합니다
+사진과 같은 품질입니다
+원래 95를 입는데 100 사이즈가 저한테는 잘 맞습니다
+가볍고 몸에 잘 맞고 겨드랑이부터 옆구리까지 매쉬 원단으로 통풍이 좋습니다
+마감도 좋고 제품의 완성도도 좋아요
+주머니도 깊어서 실용적이예요
+방수기능은 아직 확인치 못했고 스판 기능은 없습니다
+지퍼도 부드럽고 가벼운 운동이나 산책할때 입기에는 실망시키지안는 제품입니다
+강추합니다
+많이 파시고 대박나세요</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>모렉스 남성 포르테 바람막이 모자 분리형 등산복 잠바 작업복 점퍼 자켓, 239_회색, 100</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>온방바닥에 실밥 천지고 실밥정리가 전혀안되있어요 털어봐도 어디서나오는지 계속나와요 ㅠ
-허리띠는 짧아서 쓸수도 없어요
-ㅠ</t>
+          <t>https://link.coupang.com/a/cmgjvF</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>http://thumbnail10.coupangcdn.com/thumbnails/remote/292x292ex/image/vendor_inventory/f946/97b84ec7d4b48c3b6fa58a9dbf36fb7c41c152cf18eada1c4f565c6248c1.jpg</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>사용 후 솔직히 느낀대로 남겨봅니다!
+구매 시 도움 되셨으면 좋겠습니다^^
+** 나중에 재구매할 때 보기 위해서 최대한 꼼꼼히 적어둡니다. 다른분들에게 구매 시 도움 되셨으면 하는 바램 입니다 **
+주문일 24.11.14
+배송일 24.11.14
+●구매당시금액 2 8 2 0 0
+*구매사유
+아직 겨울이 오기전이라 기모 들어간 옷만 너무 많은거 같아서 편하게 막 입을 옷을 찾다가 이곳저곳 활용하기 좋아보여 바로 구매했습니다.
+*장점
+피부에 직접 닿기 때문에 제일 중요한 소재,디자인,활용도 순을 중점으로 보는데 우선 디자인이 마음에 들어 구매했습니다.
+비닐포장으로 왔고 전체적으로 마감,오염등 없이 잘 도착했습니다!
+까슬거리거나 상표 등 거슬리는것은 없었습니다.
+재질은 만지면 바스락 거리는 소리가 나고 , 냄새는 나지 않았습니다!
+다만 실밥들이 좀 붙어 있었는데 툭툭 털면 떨어지는 정도 였습니다!
+목부분의 지퍼는 부드럽게 잘 올라오고 내려가서 상황에 따라서 조절하면 될 듯 합니다!
+앞에 주머니는 꽤 깊어서 너무 무거운 물건을 넣으면 배가 부각되어보일거 같아서 간단히 카드,이어폰 등 넣기 좋을 듯 합니다.
+가운데 하단에는 조일 수 있게 되어 있는데 제 체형에는 조이지 않고 그냥 입는게 보기에도 좋고 편할꺼 같습니다!
+하의는 현재 70키로 정도 나가고 , 하체에 살이 많은 타입인데
+어제 검정 L-XL로 구매 했었는데 날씬해 보여 만족해서
+한사이즈 업해서 베이지 색상으로 또! 구매 했습니다.
+L 사이즈와 비교했을 때 우선 상의는 확실히 넉넉했고 , 손목에 시보리도 남아서 손을 걷어봤을 때 널럴해서 잘 여며서 넘기는게 아니라면 스르륵 풀려서 내려올 정도 였습니다!
+하의는 앉았다 일어났을 때 전~혀 불편함 없이 움직일 수 있어서 좋았습니다. 자주 손이 갈꺼 같습니다^^!
+아직 세탁,건조기 돌려보지는 않았는데 혹시 건조기까지 사용해서 줄어드는 상황이 오면 상품평에 추가해두겠습니다~!
+두께가 적당히 얇지도 두껍지도 않아서 날씨가 지금보다는 조금 더 추워지면 패딩조끼와 같이 잘 활용해서 입을 수 있을 듯 합니다!
+*단점
+하루차이로 한사이즈 업해서 다른색상 구매했는데 금액이 올랐습니다 ㅠㅠ
+내돈내산으로 제 상품평이 도움이 되셨다면 도움돼요 한번 부탁드립니다~^^</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>잘빠진 여성용 어반 아노락 반집업 조거 상하의 세트, S~M, 카키</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
+        <is>
+          <t>https://link.coupang.com/a/cmgjww</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>http://thumbnail10.coupangcdn.com/thumbnails/remote/292x292ex/image/vendor_inventory/9b89/ad8bbbf576af4ccf68b42d755e0223480f32ca1b1c5535c862c042243e9f.JPG</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>깔끔하고 아주편하게 입기 좋아요.
 컬러도 너무마음에들고 전반적으로 디자인이 아주깔끔해요,
@@ -468,9 +545,24 @@
 심지어가격도 너무나 착해서 부담없더라구요.</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>여성 바람막이 아웃도어 등산복 자켓, 핑크, 2XL</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
+        <is>
+          <t>https://link.coupang.com/a/cmgjxy</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>http://thumbnail8.coupangcdn.com/thumbnails/remote/292x292ex/image/vendor_inventory/ba8c/78a259c7231dc46f31f8e905dbed70e232a7641595ee1de0dbde944dfac6.jpg</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>민트스쿨 남성용 아웃도어 등산복 바람막이, 진그레이 5XL를 구매했어요. 남편이 체구가 있는 편이라 5XL 사이즈를 선택했는데, 정말 잘 맞더라고요. 색상은 호불호가 없는 진한 그레이라서 어떤 옷과도 잘 어울리고, 남편도 마음에 들어 했어요.
 이 바람막이는 소매 주머니 지퍼 부분이 정말 견고하게 만들어져 있어서 보통 저렴한 제품에서 느껴지는 싼 티가 나지 않아요. 주머니 지퍼가 튼튼하게 잘 작동하고, 디자인도 깔끔해서 실용성이 높아요. 남편이 자주 외출할 때 필요한 아이템이라 더욱 신경 써서 고른 것인데, 이렇게 만족스러운 제품을 찾게 되어 기쁘네요.
@@ -480,121 +572,63 @@
 이번에 구입한 아웃도어 바람막이는 색상과 디자인, 기능성 모두 만족스러운 제품이에요. 주름 문제는 조금 아쉽지만, 전체적인 만족도는 높아서 잘 입고 다니고 있어요.</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>민트스쿨 남성용 아웃도어 등산복 바람막이, 블랙, 3XL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>바람막이가 있긴한데....색상도 그렇고 크기고 제게 좀 큰거라서
-잘 안입게 되더라구요...저는 원래 타이트하게 딱 입는 스탈이고
-깔끔한걸 좋아해요~~
-이번에 일교차가 큰 나라로 여행을 가게 되어 바람막이가
-있는지 봤는데 제가 마음에 드는 옷이 없어 찾아보게 되었어요~
-여러 사이트도 비교해보고 봄, 가을에 입을수 있는...부담이 없는
-막 입을 정도로의 옷을 찾아보고 있었는데요.
-그 중에 디자인이나 성능이나 가성비....브랜드 모두 만족시켜주는
-바람막이가 바로 &lt;몽벨 남성 웜테크 트랙 자켓&gt;이었어요!!!
-일단 바람막이니깐 역할은 보온을 해주면서도 바람을 피해 갈 수
-있는 정도면 될 것 같았는데 몽벨 트랙자켓은 등 부분에 얇은 기모?처럼 되어 있어 덥지도 춥지도 않게 온도를 유지시켜 줄수
-있는 자켓이었습니다.
-또한 막 휘날리고 이런 소재가 아니라 어느정도 각을 잡아주는
-봄에 입으면 딱 이쁜 그런 자켓이었어요~~역할은 바람막이지만
-디자인은 또 자켓이고 완전 이쁜 그 자체였습니다^^
-겉감은 물을 튕겨내는 발수 기능이 있어 비가 오는 날에도 끄덕없이 편하게 입을수 있고, 땀과 습기를 수증기 형태로 배출하는 투습 기능도 있다고 합니다.
-등산이나 외출복에도 안성맞춤일 것 같구요.
-색상은 문안하게 블랙으로 했는데 입으니깐 영롱하게 너무 멋져서
-잘 샀다고 생각했어요 ㅋㅋㅋ
-일반 바람막이보다는 자켓형태로 되어 있다보니 무게가 조금 더
-나가는것 같고, 봄, 여름, 초겨울에도 입을수 있는 광범위하게
-디자인이 되어 있어 완전 만족하면서 입을려구요!!!
-봄에는 셔츠나 라운드티에 입어도 되고 조금 춥다고 생각되면
-그 위에 경량 베스트 하나 입고 마지막에 자켓을 입으면 딱일것
-같다는 생각이 드네요~~~
-바깥쪽 메인 지펴를 올리게 되면 그 외부에 플라켓 처리가 되어있어 단추로 딱 잠그면 지퍼 사이로 들어오는 바람을 최소화
-시켜주어 체온 유지에 도움을 주는것 같습니다.
-또한 마음에 들었던게 손목 밑단에 밴딩 처리를 하여 편안한
-착용감과 활동성을 강화시켜 주어 너무 좋았어요~~
-흘러내리지도 않고 옷맵시를 딱 잡아주어 멋져보였어요!
-앞쪽에 몽벨 브랜드 로고도 심플하게 처리 되어 있고 와펜도
-부착되어 있어 밋밋할 수 있는 바람막이를 특징있게 살려낸것도
-포인트인거 같아요~^^
-블랙 자켓이다보니 팬츠도 블랙으로 깔맞춤하게 되면 러닝할때나
-등산할때나 일상복으로도 충분히 깔끔하게 입을수 있는 바람막인거 같아서 자주 입게 될 것 같아요.
-제가 M(95)와 L(100)사이즈를 엄청 고민했었는데요.
-어깨가 조금 좁고 소매통도 작아 95를 선택해봤는데 완전
-깔맞춤이었습니다! 사이즈가 딱 맞아서 너무 기뻣어요~
-바람막이 역할이 많이 있지만 디자인은 자켓형태라서 너무
-헐거워 보이면 좀 멋없을것 같아 95했는데 예상적중했네요!
-다만...상품 페이지에는 제조국이 베트남이었는데,
-막상 제품 안쪽 라벨에는 제조국이 중국이네요...
-그게 좀 실망스럽긴 하지만....나머지 부분인 바람막이의 역할,
-기능성, 활동성, 브랜드 이미지, 가성비 측면 등 모든 부분이
-만족되어 기쁘게 입을려고 합니다~~~
-구매시 제조국에 조금 예민하신 분들은 참고 부탁드립니다...
-이상 내돈내산 솔직한 후기였으며,
-구매시 긴 후기가 도움이 되셨다면 &lt;&lt;도움이 돼요&gt;&gt;버튼을
-눌러주시면 솔직한 후기 작성에 힘이 날 것 같습니다^^
-감사합니다. 좋은 하루 되세요^______^</t>
+          <t>https://link.coupang.com/a/cmgjy5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>http://thumbnail7.coupangcdn.com/thumbnails/remote/292x292ex/image/vendor_inventory/169b/897ec8656a9c0c399c29cd115b71b0726531590881750add0905a15891c7.jpg</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>잘 받았습니다.
+퀄리티가 너무 좋아서 특별히 착용 소감을 적어봤습니다.
+더 많은 친구들이 이 겨울 자켓을 구매할 수 있기를 바랍니다.
+이 겨울 재킷을 처음 입었을 때 사방에 감싸인 포근함이 순간적으로 온몸에 훈훈한 온기가 느껴졌습니다.
+저는 아웃도어 활동과 자동차 여행을 즐기는 사람으로서 실용적이면서도 편안한 외투가 여행에서 얼마나 중요한지 잘 알고 있습니다.
+이 재킷은 외부에 바람막이 원단을 사용함으로써 방풍,방수 효과가 뛰어나며 그로인해 방한과보온성 또한 뛰어납니다.
+이 재킷은 마치 제 개인 보호막처럼 빗물이 때려도 안으로 전혀 스며들지 않아 항상 건조하고 편안함을 유지시켜 줍니다.
+눈내리는날 우산없이 눈내리는 풍경을 마음껏 즐길 수 있을겁니다.
+그리고 그 방풍기능은 더욱 절 감탄하게 합니다.
+찬바람이 부는 겨울날에도 따뜻한 온기가 나를 감싸고 있는 것을 느낄 수 있습니다.
+마치 따뜻한 품에 안겨 있는 것 같습니다.
+창문을 열고 운전할 때도 이 재킷은 역시나 훌륭합니다.
+재킷의 커팅 디자인이 매우 인간적이며, 큰 사이즈의 선택이 내 체형에 완벽하게 맞아떨어져서 운전석에서 아무런 구속 없이 자유롭게 움직일 수 있게 해줍니다.
+또한 가벼운 소재와 스크레치 방지 기능으로 장시간 주행 후에도 의류가 손상되거나 주행 안전에 지장을 줄 염려 없이 산뜻하고 편안함을 유지시켜 줍니다.
+더욱 놀라운 것은 이 재킷의 디자인이 매우 스타일리시하다는 것입니다.
+단순히 실용적인 아웃도어 아이템이 아니라 전체적인 이미지를 높일 수 있는 패션 아이템입니다.
+캐주얼 팬츠나 청바지에 코디하기에도 부담 없이 다양한 장소를 소화할 수 있어 아웃도어 생활과 일상생활에서도 자신감과 멋을 유지할 수 있습니다.
+이제 저는 거의 매일 이 옷을 입고 이 추운 겨울을 함께 할 것입니다.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>남자패딩 등산 코트 빅사이즈 바람막이 아웃도어자켓 방한 아우터 방수 방풍 보드복 겨울 스키복, 다크그레이 dark..., S</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>바람막이가 있긴한데....색상도 그렇고 크기고 제게 좀 큰거라서
-잘 안입게 되더라구요...저는 원래 타이트하게 딱 입는 스탈이고
-깔끔한걸 좋아해요~~
-이번에 일교차가 큰 나라로 여행을 가게 되어 바람막이가
-있는지 봤는데 제가 마음에 드는 옷이 없어 찾아보게 되었어요~
-여러 사이트도 비교해보고 봄, 가을에 입을수 있는...부담이 없는
-막 입을 정도로의 옷을 찾아보고 있었는데요.
-그 중에 디자인이나 성능이나 가성비....브랜드 모두 만족시켜주는
-바람막이가 바로 &lt;몽벨 남성 웜테크 트랙 자켓&gt;이었어요!!!
-일단 바람막이니깐 역할은 보온을 해주면서도 바람을 피해 갈 수
-있는 정도면 될 것 같았는데 몽벨 트랙자켓은 등 부분에 얇은 기모?처럼 되어 있어 덥지도 춥지도 않게 온도를 유지시켜 줄수
-있는 자켓이었습니다.
-또한 막 휘날리고 이런 소재가 아니라 어느정도 각을 잡아주는
-봄에 입으면 딱 이쁜 그런 자켓이었어요~~역할은 바람막이지만
-디자인은 또 자켓이고 완전 이쁜 그 자체였습니다^^
-겉감은 물을 튕겨내는 발수 기능이 있어 비가 오는 날에도 끄덕없이 편하게 입을수 있고, 땀과 습기를 수증기 형태로 배출하는 투습 기능도 있다고 합니다.
-등산이나 외출복에도 안성맞춤일 것 같구요.
-색상은 문안하게 블랙으로 했는데 입으니깐 영롱하게 너무 멋져서
-잘 샀다고 생각했어요 ㅋㅋㅋ
-일반 바람막이보다는 자켓형태로 되어 있다보니 무게가 조금 더
-나가는것 같고, 봄, 여름, 초겨울에도 입을수 있는 광범위하게
-디자인이 되어 있어 완전 만족하면서 입을려구요!!!
-봄에는 셔츠나 라운드티에 입어도 되고 조금 춥다고 생각되면
-그 위에 경량 베스트 하나 입고 마지막에 자켓을 입으면 딱일것
-같다는 생각이 드네요~~~
-바깥쪽 메인 지펴를 올리게 되면 그 외부에 플라켓 처리가 되어있어 단추로 딱 잠그면 지퍼 사이로 들어오는 바람을 최소화
-시켜주어 체온 유지에 도움을 주는것 같습니다.
-또한 마음에 들었던게 손목 밑단에 밴딩 처리를 하여 편안한
-착용감과 활동성을 강화시켜 주어 너무 좋았어요~~
-흘러내리지도 않고 옷맵시를 딱 잡아주어 멋져보였어요!
-앞쪽에 몽벨 브랜드 로고도 심플하게 처리 되어 있고 와펜도
-부착되어 있어 밋밋할 수 있는 바람막이를 특징있게 살려낸것도
-포인트인거 같아요~^^
-블랙 자켓이다보니 팬츠도 블랙으로 깔맞춤하게 되면 러닝할때나
-등산할때나 일상복으로도 충분히 깔끔하게 입을수 있는 바람막인거 같아서 자주 입게 될 것 같아요.
-제가 M(95)와 L(100)사이즈를 엄청 고민했었는데요.
-어깨가 조금 좁고 소매통도 작아 95를 선택해봤는데 완전
-깔맞춤이었습니다! 사이즈가 딱 맞아서 너무 기뻣어요~
-바람막이 역할이 많이 있지만 디자인은 자켓형태라서 너무
-헐거워 보이면 좀 멋없을것 같아 95했는데 예상적중했네요!
-다만...상품 페이지에는 제조국이 베트남이었는데,
-막상 제품 안쪽 라벨에는 제조국이 중국이네요...
-그게 좀 실망스럽긴 하지만....나머지 부분인 바람막이의 역할,
-기능성, 활동성, 브랜드 이미지, 가성비 측면 등 모든 부분이
-만족되어 기쁘게 입을려고 합니다~~~
-구매시 제조국에 조금 예민하신 분들은 참고 부탁드립니다...
-이상 내돈내산 솔직한 후기였으며,
-구매시 긴 후기가 도움이 되셨다면 &lt;&lt;도움이 돼요&gt;&gt;버튼을
-눌러주시면 솔직한 후기 작성에 힘이 날 것 같습니다^^
-감사합니다. 좋은 하루 되세요^______^</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+          <t>https://link.coupang.com/a/cmgjBD</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>http://thumbnail7.coupangcdn.com/thumbnails/remote/292x292ex/image/vendor_inventory/2a27/f75c9f3bf68a4c3fec9b6fc75d14d6d7bd11d247085aead2de23ec3a7489.jpg</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>✨maomaodian바람막이 등산복 점퍼 남성 방수 아웃도어 봄 가을 탈부착 J1
 ✔️세 가지 컬러
@@ -623,9 +657,24 @@
 ⭕️재 후기가 도움이 되었다면‘도움이 돼요‘를 꾸욱 눌러주세요.</t>
         </is>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>maomaodian바람막이 등산복 점퍼 남성 방수 아웃도어 봄 가을 탈부착 J1, 블랙, L(95)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>https://link.coupang.com/a/cmgjC7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>http://thumbnail8.coupangcdn.com/thumbnails/remote/292x292ex/image/vendor_inventory/2448/4ab510406faa34aa4307bac3697ff868cd0cd59d78f8a7369b3b98b89e20.jpg</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>남편이 저녁때 조금 쌀쌀할 때 입을만한 옷 필요하다고 구매해달라고 해서 구매하게 되었답니당~^^♡
 검정색 회색 카키색 있는데 회색이 젤 무난해보이더라구요.
@@ -661,21 +710,55 @@
 진짜 이쁜옷 잘 산듯 해요.</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>맨하트 춘추 아웃도어 자켓 등산복 일상복 작업복 빅사이즈 MHWF-59, 100, 블랙</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://link.coupang.com/a/cmgjD7</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>http://thumbnail8.coupangcdn.com/thumbnails/remote/292x292ex/image/vendor_inventory/a91c/9e3d33d7cdb1dce0bae29598b4c2acd0a7f7ca170087fc6e59da70ef2751.jpg</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>작업복으로 입으려고 구매했습니다. 가랭이부분,엉덩이 부분,허리 부분, 지퍼 부분이 특히 중요한데요 박음질이 엉망입니다. 같은 사이즈인데 바지밑단의 넓이와 길이가 다릅니다. 일하다 가랭이나 엉덩이부분 터질까봐 걱정이네요.
+재질,디자인은 마음에 듭니다. 박음질 견고하고 깔끔하게 좀 만들어주세요.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>워킹맨 아울렛 남성 1+1 봄 가을 시즌 다용도 멀티 스판 캠핑바지 낚시복 작업복 근무복 캠핑복 B128, 카키색+카키색, 34</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>빠른 배송 감사합니다
-인터넷 쇼핑으로 의류를 구매하고 실망한 경험이 있었는데 만족합니다
-사진과 같은 품질입니다
-원래 95를 입는데 100 사이즈가 저한테는 잘 맞습니다
-가볍고 몸에 잘 맞고 겨드랑이부터 옆구리까지 매쉬 원단으로 통풍이 좋습니다
-마감도 좋고 제품의 완성도도 좋아요
-주머니도 깊어서 실용적이예요
-방수기능은 아직 확인치 못했고 스판 기능은 없습니다
-지퍼도 부드럽고 가벼운 운동이나 산책할때 입기에는 실망시키지안는 제품입니다
-강추합니다
-많이 파시고 대박나세요</t>
+          <t>https://link.coupang.com/a/cmggzt</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>http://thumbnail8.coupangcdn.com/thumbnails/remote/292x292ex/image/vendor_inventory/a91c/9e3d33d7cdb1dce0bae29598b4c2acd0a7f7ca170087fc6e59da70ef2751.jpg</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>작업복으로 입으려고 구매했습니다. 가랭이부분,엉덩이 부분,허리 부분, 지퍼 부분이 특히 중요한데요 박음질이 엉망입니다. 같은 사이즈인데 바지밑단의 넓이와 길이가 다릅니다. 일하다 가랭이나 엉덩이부분 터질까봐 걱정이네요.
+재질,디자인은 마음에 듭니다. 박음질 견고하고 깔끔하게 좀 만들어주세요.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>워킹맨 아울렛 남성 1+1 봄 가을 시즌 다용도 멀티 스판 캠핑바지 낚시복 작업복 근무복 캠핑복 B128, 카키색+카키색, 34</t>
         </is>
       </c>
     </row>

</xml_diff>